<commit_message>
Merge in changes from 1.8
</commit_message>
<xml_diff>
--- a/openpyxl/tests/test_data/genuine/empty.xlsx
+++ b/openpyxl/tests/test_data/genuine/empty.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="24030"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="100" windowWidth="24800" windowHeight="12260" activeTab="1"/>
+    <workbookView xWindow="180" yWindow="0" windowWidth="29300" windowHeight="19100" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1 - Text" sheetId="1" r:id="rId1"/>
@@ -75,11 +75,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Prozent" xfId="1" builtinId="5"/>
@@ -407,8 +408,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D1:AA30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="AA1" sqref="AA1:AA30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.875" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -508,6 +509,9 @@
       <c r="D9">
         <v>9</v>
       </c>
+      <c r="G9" s="4" t="b">
+        <v>1</v>
+      </c>
       <c r="K9" s="1">
         <v>0.09</v>
       </c>
@@ -518,6 +522,9 @@
     <row r="10" spans="4:27">
       <c r="D10">
         <v>10</v>
+      </c>
+      <c r="G10" t="b">
+        <v>0</v>
       </c>
       <c r="K10" s="1">
         <v>0.1</v>

</xml_diff>